<commit_message>
Backup reminder system updates and new scripts
</commit_message>
<xml_diff>
--- a/data/rem_conference_deadlines.xlsx
+++ b/data/rem_conference_deadlines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cesarlandin/Projects/remindr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cesarlandin/Projects/remindr/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A221E792-A0CB-9847-B958-0C9F1B004715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8281C6A1-E9CF-D649-995A-75EDB4BF65AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-2280" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rem_conference_deadlines" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>deadline</t>
   </si>
@@ -46,12 +46,6 @@
     <t>complete</t>
   </si>
   <si>
-    <t>2022_06_01</t>
-  </si>
-  <si>
-    <t>20th IO conference on Augus 16-18 at Berlin</t>
-  </si>
-  <si>
     <t>io-conference@uni.edu</t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>io-conference.edu</t>
   </si>
   <si>
-    <t>2022_07_06</t>
-  </si>
-  <si>
     <t>US University Finance Conference on September 20</t>
   </si>
   <si>
@@ -76,7 +67,31 @@
     <t>https://usconf.uni.edu</t>
   </si>
   <si>
-    <t>2022_08_06</t>
+    <t>date</t>
+  </si>
+  <si>
+    <t>20th IO conference on August 16-18 at Berlin</t>
+  </si>
+  <si>
+    <t>2023_08_16</t>
+  </si>
+  <si>
+    <t>2023_09_20</t>
+  </si>
+  <si>
+    <t>2023_07_06</t>
+  </si>
+  <si>
+    <t>2023_06_01</t>
+  </si>
+  <si>
+    <t>timezone</t>
+  </si>
+  <si>
+    <t>CST6CDT</t>
+  </si>
+  <si>
+    <t>EST</t>
   </si>
 </sst>
 </file>
@@ -918,20 +933,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="44.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -939,70 +954,88 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3">
+      <c r="J3">
         <v>0</v>
       </c>
     </row>

</xml_diff>